<commit_message>
Add missing borders in buglist
</commit_message>
<xml_diff>
--- a/Project1/buglist.xlsx
+++ b/Project1/buglist.xlsx
@@ -1,14 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nik312123/git/repo-Team19/Project1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ED8A72-0CB0-4848-9FD1-89565A428603}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$4</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -33,30 +43,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -77,55 +91,65 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -315,28 +339,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.71"/>
-    <col customWidth="1" min="2" max="2" width="30.43"/>
-    <col customWidth="1" min="3" max="3" width="35.43"/>
-    <col customWidth="1" min="4" max="4" width="54.29"/>
-    <col customWidth="1" min="5" max="5" width="51.86"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="54.33203125" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -353,27 +382,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -381,10 +410,9 @@
       <c r="E4" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$4"/>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>